<commit_message>
Se separa el preprocesamiento
</commit_message>
<xml_diff>
--- a/Data_Direcciones.xlsx
+++ b/Data_Direcciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42A5BE9-B6AE-4BC2-B633-0D531B7E10C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511CE7E3-7AB0-4A1C-8397-41EDDB62D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
     <t>E/S ZARATE</t>
   </si>
   <si>
-    <t>Malecón Checa Eguiguren, San Juan de Lurigancho 15401, Perú</t>
+    <t>Av. Malecón Checa, San Juan de Lurigancho 15401, Perú</t>
   </si>
   <si>
     <t>P371</t>
@@ -922,7 +922,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se cambia el convertidor de localización por una clase
</commit_message>
<xml_diff>
--- a/Data_Direcciones.xlsx
+++ b/Data_Direcciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511CE7E3-7AB0-4A1C-8397-41EDDB62D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4921F7EF-2368-472E-9B78-1BFC61090687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,7 +922,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>